<commit_message>
Spindrehkurve und noch mehr
</commit_message>
<xml_diff>
--- a/NMR/Auswertung Uli.xlsx
+++ b/NMR/Auswertung Uli.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="9315" windowHeight="9270"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="9315" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Frequenz</t>
   </si>
@@ -72,7 +72,40 @@
     <t>y</t>
   </si>
   <si>
-    <t>[]</t>
+    <t>Verschiebung der Spindrehkurven</t>
+  </si>
+  <si>
+    <t>max1</t>
+  </si>
+  <si>
+    <t>max2</t>
+  </si>
+  <si>
+    <t>kl-fit</t>
+  </si>
+  <si>
+    <t>k=</t>
+  </si>
+  <si>
+    <t>l=</t>
+  </si>
+  <si>
+    <t>Einstrahlspule</t>
+  </si>
+  <si>
+    <t>2,6 cm</t>
+  </si>
+  <si>
+    <t>1,7cm</t>
+  </si>
+  <si>
+    <t>Durchmesser</t>
+  </si>
+  <si>
+    <t>Länge</t>
+  </si>
+  <si>
+    <t>Halbwertsbreite</t>
   </si>
 </sst>
 </file>
@@ -411,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,9 +794,76 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>3.4826099999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>4.5535699999999998E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f>(B42-B41)/2</f>
+        <v>5.3547999999999998E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47">
+        <v>-1.58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QHE: Zusammenfassung und Abstact überarbeitet
</commit_message>
<xml_diff>
--- a/NMR/Auswertung Uli.xlsx
+++ b/NMR/Auswertung Uli.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>Frequenz</t>
   </si>
@@ -142,6 +142,27 @@
   </si>
   <si>
     <t>Mittelwert</t>
+  </si>
+  <si>
+    <t>relative Spinaufspaltung</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>E_F in meV</t>
+  </si>
+  <si>
+    <t>k_F</t>
+  </si>
+  <si>
+    <t>v_F</t>
+  </si>
+  <si>
+    <t>(rel fehler)</t>
   </si>
 </sst>
 </file>
@@ -487,15 +508,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1146,10 +1170,10 @@
     </row>
     <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>3.5840000000000001</v>
+        <v>3.5619000000000001</v>
       </c>
       <c r="B63">
-        <v>7.0000000000000007E-2</v>
+        <v>8.8999999999999999E-3</v>
       </c>
       <c r="C63" s="1">
         <v>3.45</v>
@@ -1165,26 +1189,23 @@
       </c>
       <c r="H63">
         <f>(E63*E69+C63*C69+A63*A69)/F69</f>
-        <v>3.5666977886977889</v>
+        <v>3.5604860536965317</v>
       </c>
       <c r="I63">
         <f>SQRT((B63^2*A69^2+D63^2*C69^2+F63^2*E69^2))/F69</f>
-        <v>6.0770726123055452E-2</v>
-      </c>
-      <c r="J63">
-        <v>6.0999999999999999E-2</v>
+        <v>1.3683962604856419E-2</v>
       </c>
       <c r="L63">
         <f>SQRT(B63^2+D63^2+F63^2)/3</f>
-        <v>7.3181661333667172E-2</v>
+        <v>6.9425587662058877E-2</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>3.6339999999999999</v>
+        <v>3.5714999999999999</v>
       </c>
       <c r="B64">
-        <v>7.0999999999999994E-2</v>
+        <v>9.4000000000000004E-3</v>
       </c>
       <c r="C64" s="1">
         <v>3.37</v>
@@ -1200,22 +1221,19 @@
       </c>
       <c r="H64">
         <f t="shared" ref="H64:H66" si="5">(E64*E70+C64*C70+A64*A70)/F70</f>
-        <v>3.5836282836263087</v>
+        <v>3.5667553296812091</v>
       </c>
       <c r="I64">
         <f t="shared" ref="I64:I66" si="6">SQRT((B64^2*A70^2+D64^2*C70^2+F64^2*E70^2))/F70</f>
-        <v>6.6066295073612794E-2</v>
-      </c>
-      <c r="J64">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+        <v>1.4614571661250431E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>3.637</v>
+        <v>3.556</v>
       </c>
       <c r="B65">
-        <v>7.0999999999999994E-2</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="C65" s="1">
         <v>3.41</v>
@@ -1231,22 +1249,19 @@
       </c>
       <c r="H65">
         <f t="shared" si="5"/>
-        <v>3.588690242305173</v>
+        <v>3.5538474481211439</v>
       </c>
       <c r="I65">
         <f t="shared" si="6"/>
-        <v>6.3890405034487854E-2</v>
-      </c>
-      <c r="J65">
-        <v>6.4000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+        <v>1.4642613108667905E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>3.6360000000000001</v>
+        <v>3.5541999999999998</v>
       </c>
       <c r="B66">
-        <v>7.0999999999999994E-2</v>
+        <v>9.7000000000000003E-3</v>
       </c>
       <c r="C66" s="1">
         <v>3.42</v>
@@ -1262,17 +1277,14 @@
       </c>
       <c r="H66">
         <f t="shared" si="5"/>
-        <v>3.59385939444214</v>
+        <v>3.5533712068242203</v>
       </c>
       <c r="I66">
         <f t="shared" si="6"/>
-        <v>6.5032724742916881E-2</v>
-      </c>
-      <c r="J66">
-        <v>6.5000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.4977722250460138E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>39</v>
       </c>
@@ -1281,17 +1293,17 @@
       </c>
       <c r="H68">
         <f>SUM(H63:H66)/4</f>
-        <v>3.5832189272678527</v>
-      </c>
-      <c r="J68">
-        <f>SQRT(J63^2+J64^2+J65^2+J66^2)/2</f>
-        <v>6.4027337911239129E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.5586150095807763</v>
+      </c>
+      <c r="I68">
+        <f>SQRT(I63^2+I64^2+I65^2+I66^2)/2</f>
+        <v>1.4487708754967044E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <f>1/B63</f>
-        <v>14.285714285714285</v>
+        <v>112.35955056179776</v>
       </c>
       <c r="C69">
         <f>1/D63</f>
@@ -1303,13 +1315,13 @@
       </c>
       <c r="F69">
         <f>E69+C69+A69</f>
-        <v>28.501400560224088</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+        <v>126.57523683630757</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" ref="A70:A72" si="7">1/B64</f>
-        <v>14.084507042253522</v>
+        <v>106.38297872340425</v>
       </c>
       <c r="C70">
         <f t="shared" ref="C70:C72" si="8">1/D64</f>
@@ -1321,13 +1333,13 @@
       </c>
       <c r="F70">
         <f t="shared" ref="F70:F72" si="10">E70+C70+A70</f>
-        <v>26.216859983429991</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+        <v>118.51533166458071</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="7"/>
-        <v>14.084507042253522</v>
+        <v>105.26315789473685</v>
       </c>
       <c r="C71">
         <f t="shared" si="8"/>
@@ -1339,13 +1351,13 @@
       </c>
       <c r="F71">
         <f t="shared" si="10"/>
-        <v>27.109717126287137</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+        <v>118.28836797877047</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="7"/>
-        <v>14.084507042253522</v>
+        <v>103.09278350515464</v>
       </c>
       <c r="C72">
         <f t="shared" si="8"/>
@@ -1357,7 +1369,258 @@
       </c>
       <c r="F72">
         <f t="shared" si="10"/>
-        <v>26.633526650096659</v>
+        <v>115.64180311299778</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>32</v>
+      </c>
+      <c r="B77">
+        <v>7.8600000000000003E-2</v>
+      </c>
+      <c r="C77">
+        <f>B78-B77</f>
+        <v>8.6400000000000005E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="D78">
+        <f>B78</f>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E78">
+        <f>(C77+C79)/2</f>
+        <v>8.1199999999999994E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="C79">
+        <f>B79-B78</f>
+        <v>7.5999999999999984E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f>D82-D78</f>
+        <v>0.39769999999999994</v>
+      </c>
+      <c r="G80">
+        <f>SQRT(E78^2+E82^2)</f>
+        <v>0.11294109083942831</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81">
+        <v>0.48139999999999999</v>
+      </c>
+      <c r="C81">
+        <f>B82-B81</f>
+        <v>8.1299999999999983E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>43</v>
+      </c>
+      <c r="B82">
+        <v>0.56269999999999998</v>
+      </c>
+      <c r="D82">
+        <f>B82</f>
+        <v>0.56269999999999998</v>
+      </c>
+      <c r="E82">
+        <f>(C81+C83)/2</f>
+        <v>7.8499999999999986E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83">
+        <v>0.63839999999999997</v>
+      </c>
+      <c r="C83">
+        <f>B83-B82</f>
+        <v>7.569999999999999E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>44</v>
+      </c>
+      <c r="B85" t="s">
+        <v>45</v>
+      </c>
+      <c r="C85" t="s">
+        <v>46</v>
+      </c>
+      <c r="D85" t="s">
+        <v>47</v>
+      </c>
+      <c r="E85" t="s">
+        <v>48</v>
+      </c>
+      <c r="F85" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <f>H63*10^15</f>
+        <v>3560486053696531.5</v>
+      </c>
+      <c r="B86">
+        <f>(1.0546*10^-34)^2*3.1415926/(0.067*9.109*10^-31)/(1.602*10^-19)*A86</f>
+        <v>1.2724088225934663E-2</v>
+      </c>
+      <c r="C86">
+        <f>SQRT(A86*2*3.1415926)*10^-9</f>
+        <v>0.14957002800491967</v>
+      </c>
+      <c r="D86">
+        <f>(1.0546*10^-34)*SQRT(2*3.1415926*A86)/(0.067*9.109*10^-31)/1000</f>
+        <v>258.45613004358205</v>
+      </c>
+      <c r="E86">
+        <f>I63/H63</f>
+        <v>3.843284989320375E-3</v>
+      </c>
+      <c r="F86">
+        <f>B86*E86</f>
+        <v>4.8902297281522811E-5</v>
+      </c>
+      <c r="G86">
+        <f>C86*E86/2</f>
+        <v>2.8742012174176796E-4</v>
+      </c>
+      <c r="H86">
+        <f>E86*D86/2</f>
+        <v>0.49666028249716682</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f t="shared" ref="A87:A89" si="11">H64*10^15</f>
+        <v>3566755329681209</v>
+      </c>
+      <c r="B87">
+        <f t="shared" ref="B87:B89" si="12">(1.0546*10^-34)^2*3.1415926/(0.067*9.109*10^-31)/(1.602*10^-19)*A87</f>
+        <v>1.2746492700924518E-2</v>
+      </c>
+      <c r="C87">
+        <f t="shared" ref="C87:C89" si="13">SQRT(A87*2*3.1415926)*10^-9</f>
+        <v>0.1497016509577436</v>
+      </c>
+      <c r="D87">
+        <f t="shared" ref="D87:D89" si="14">(1.0546*10^-34)*SQRT(2*3.1415926*A87)/(0.067*9.109*10^-31)/1000</f>
+        <v>258.68357373310698</v>
+      </c>
+      <c r="E87">
+        <f t="shared" ref="E87:E89" si="15">I64/H64</f>
+        <v>4.0974415989886975E-3</v>
+      </c>
+      <c r="F87">
+        <f t="shared" ref="F87:F89" si="16">B87*E87</f>
+        <v>5.2228009433973915E-5</v>
+      </c>
+      <c r="G87">
+        <f t="shared" ref="G87:G89" si="17">C87*E87/2</f>
+        <v>3.0669688603577239E-4</v>
+      </c>
+      <c r="H87">
+        <f t="shared" ref="H87:H89" si="18">E87*D87/2</f>
+        <v>0.52997041799454625</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <f t="shared" si="11"/>
+        <v>3553847448121144</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="12"/>
+        <v>1.2700363879942432E-2</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="13"/>
+        <v>0.14943052462295828</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="14"/>
+        <v>258.21506901878536</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="15"/>
+        <v>4.1202143092577579E-3</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="16"/>
+        <v>5.2328220990919186E-5</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="17"/>
+        <v>3.0784289289570319E-4</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="18"/>
+        <v>0.53195071111858949</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="11"/>
+        <v>3553371206824220.5</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="12"/>
+        <v>1.269866193919965E-2</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="13"/>
+        <v>0.14942051190122485</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="14"/>
+        <v>258.19776709442965</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="15"/>
+        <v>4.2150739055057196E-3</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="16"/>
+        <v>5.3525798574759102E-5</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="17"/>
+        <v>3.1490925033107986E-4</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="18"/>
+        <v>0.54416133526978694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>